<commit_message>
solucionario + plot na aula07
</commit_message>
<xml_diff>
--- a/Dados/output_excel.xlsx
+++ b/Dados/output_excel.xlsx
@@ -558,7 +558,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>[46]</t>
+          <t>Comparable in size to the May 2024 storms.[46]</t>
         </is>
       </c>
     </row>
@@ -726,7 +726,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>[61] [62]</t>
+          <t>[61][62]</t>
         </is>
       </c>
     </row>
@@ -746,7 +746,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>[61] [62]</t>
+          <t>[61][62]</t>
         </is>
       </c>
     </row>
@@ -766,7 +766,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>[61] [63]</t>
+          <t>[61][63]</t>
         </is>
       </c>
     </row>
@@ -908,7 +908,11 @@
           <t>Bastille Day solar storm</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr"/>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Caused by an X8-class solar flare aimed directly at Earth</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1034,7 +1038,7 @@
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Triggered by an X8.2 class solar flare[87][88][89][90]</t>
+          <t>Triggered by an X13 class solar flare[87][88][89][90]</t>
         </is>
       </c>
     </row>
@@ -1070,7 +1074,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>X1.2(X1.3)-class flares[93] and X4.5-class flare[94]. The flares with a magnitude of 6–7 occurred between 30 April and 4 May 2024. On 5 May the strength of the solar storm reached 5 points, which is considered strong according to the K-index. The rapidly growing sunspot AR3663 became the most active spot of the 25th solar cycle. On 5 May alone, it emitted two X-class (strongest) flares and six M-class (medium) flares. Each of these flares resulted in a short-term but profound disconnection of the Earth's radio signal, resulting in signal loss at frequencies below 30 MHz[95] An extreme (G5) geomagnetic storm alert was issued by the National Oceanic and Atmospheric Administration (NOAA) – the first since October 2003[96][97]</t>
+          <t>X1.2(X1.3)-class flares[93] and X4.5-class flare.[94] The flares with a magnitude of 6–7 occurred between 30 April and 4 May 2024. On 5 May the strength of the solar storm reached 5 points, which is considered strong according to the K-index. The rapidly growing sunspot AR3663 became the most active spot of the 25th solar cycle. On 5 May alone, it emitted two X-class (strongest) flares and six M-class (medium) flares. Each of these flares resulted in a short-term but profound disconnection of the Earth's radio signal, resulting in signal loss at frequencies below 30 MHz.[95] An extreme (G5) geomagnetic storm alert was issued by the National Oceanic and Atmospheric Administration (NOAA) – the first since October 2003.[96][97]</t>
         </is>
       </c>
     </row>

</xml_diff>